<commit_message>
Function,procedures and methods for user input Get random num for game Player movement function+refactoring
</commit_message>
<xml_diff>
--- a/GoldenOracule1994/SuperAdventure/Text/QualitiesAndArsenal.xlsx
+++ b/GoldenOracule1994/SuperAdventure/Text/QualitiesAndArsenal.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="19095" windowHeight="8460" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="19095" windowHeight="8460"/>
   </bookViews>
   <sheets>
     <sheet name="Qualities" sheetId="1" r:id="rId1"/>
@@ -570,7 +570,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
@@ -1074,13 +1074,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:D17"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E17" sqref="C1:E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1096,7 +1097,7 @@
       <c r="D1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="8" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1111,6 +1112,7 @@
       <c r="D2" s="1">
         <v>6</v>
       </c>
+      <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
@@ -1123,6 +1125,7 @@
       <c r="D3" s="1">
         <v>3</v>
       </c>
+      <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
@@ -1135,6 +1138,7 @@
       <c r="D4" s="1">
         <v>3</v>
       </c>
+      <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
@@ -1147,6 +1151,7 @@
       <c r="D5" s="1">
         <v>2</v>
       </c>
+      <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
@@ -1159,6 +1164,7 @@
       <c r="D6" s="1">
         <v>1</v>
       </c>
+      <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
@@ -1171,6 +1177,7 @@
       <c r="D7" s="1">
         <v>1</v>
       </c>
+      <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
@@ -1183,6 +1190,7 @@
       <c r="D8" s="1">
         <v>1</v>
       </c>
+      <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
@@ -1195,7 +1203,7 @@
       <c r="D9" s="1">
         <v>4</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="1">
         <v>1</v>
       </c>
     </row>
@@ -1210,7 +1218,7 @@
       <c r="D10" s="1">
         <v>2</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="1">
         <v>2</v>
       </c>
     </row>
@@ -1225,7 +1233,7 @@
       <c r="D11" s="1">
         <v>1</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="1">
         <v>2</v>
       </c>
     </row>
@@ -1240,6 +1248,7 @@
       <c r="D12" s="1">
         <v>1</v>
       </c>
+      <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="1" t="s">
@@ -1252,6 +1261,7 @@
       <c r="D13" s="1">
         <v>1</v>
       </c>
+      <c r="E13" s="1"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="1" t="s">
@@ -1264,6 +1274,7 @@
       <c r="D14" s="1">
         <v>1</v>
       </c>
+      <c r="E14" s="1"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="1" t="s">
@@ -1276,6 +1287,7 @@
       <c r="D15" s="1">
         <v>1</v>
       </c>
+      <c r="E15" s="1"/>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="1" t="s">
@@ -1288,8 +1300,9 @@
       <c r="D16" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" s="1" t="s">
         <v>1</v>
       </c>
@@ -1300,6 +1313,7 @@
       <c r="D17" s="8">
         <v>1</v>
       </c>
+      <c r="E17" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>